<commit_message>
Composer update to PHP 8.2
</commit_message>
<xml_diff>
--- a/data/BuriedTreasureShows.xlsx
+++ b/data/BuriedTreasureShows.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18165" windowHeight="5655"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18170" windowHeight="5660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Show #</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Listener selected set</t>
   </si>
   <si>
-    <t>Steve Ferrone</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
@@ -109,6 +106,30 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Steve Ferrone guest appearance, Dentist Paul Grinder whistle</t>
+  </si>
+  <si>
+    <t>Expensive Left Banke CD</t>
+  </si>
+  <si>
+    <t>Tom Petty plays Tom Petty</t>
+  </si>
+  <si>
+    <t>Rick's is also a tire shop</t>
+  </si>
+  <si>
+    <t>Letters: Uncle Jimmy shaving his legs</t>
+  </si>
+  <si>
+    <t>Letter from Valdosta GA</t>
+  </si>
+  <si>
+    <t>Crate of chickens</t>
+  </si>
+  <si>
+    <t>Monkey story</t>
   </si>
 </sst>
 </file>
@@ -436,16 +457,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D161"/>
+  <dimension ref="A1:D163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B156" sqref="B156"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="66.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.26953125" customWidth="1"/>
+    <col min="4" max="4" width="66.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
@@ -459,7 +480,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1">
@@ -488,6 +509,7 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1">
       <c r="A7" s="2">
@@ -495,6 +517,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1">
       <c r="A8" s="2">
@@ -502,6 +525,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1">
       <c r="A9" s="2">
@@ -509,7 +533,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -519,6 +543,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1">
       <c r="A11" s="2">
@@ -526,6 +551,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1">
       <c r="A12" s="2">
@@ -533,7 +559,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -543,6 +569,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1">
       <c r="A14" s="2">
@@ -550,6 +577,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" s="1" customFormat="1">
       <c r="A15" s="2">
@@ -557,6 +585,9 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:4" s="1" customFormat="1">
       <c r="A16" s="2">
@@ -564,6 +595,9 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1">
       <c r="A17" s="2">
@@ -571,6 +605,7 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1">
       <c r="A18" s="2">
@@ -578,6 +613,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1">
       <c r="A19" s="2">
@@ -585,6 +621,7 @@
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
@@ -592,6 +629,9 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
@@ -599,6 +639,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
@@ -606,8 +647,8 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" t="s">
-        <v>27</v>
+      <c r="D22" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -616,7 +657,7 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -626,6 +667,7 @@
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
@@ -633,6 +675,7 @@
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
@@ -640,6 +683,7 @@
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
@@ -720,6 +764,9 @@
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
+      <c r="D37" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
@@ -760,104 +807,107 @@
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="2">
-        <v>46</v>
-      </c>
-      <c r="B43" s="2">
-        <v>3</v>
-      </c>
-      <c r="C43" s="2">
-        <v>1</v>
+      <c r="A43">
+        <v>45</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <v>47</v>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="B44" s="2">
+        <v>3</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45" s="2">
         <v>3</v>
       </c>
       <c r="C45" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46" s="2">
         <v>3</v>
       </c>
       <c r="C46" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -867,7 +917,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -877,7 +927,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -887,7 +937,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -897,28 +947,28 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -928,7 +978,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -938,14 +988,14 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:4">
       <c r="A65" s="2">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B65" s="2">
         <v>4</v>
@@ -954,86 +1004,89 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:4">
       <c r="A66" s="2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:4">
       <c r="A67" s="2">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:4">
       <c r="A68" s="2">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:4">
       <c r="A69" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:4">
       <c r="A70" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
-    </row>
-    <row r="71" spans="1:3">
+      <c r="D70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="2">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:4">
       <c r="A72" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:4">
       <c r="A73" s="2">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:4">
       <c r="A74" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:4">
       <c r="A75" s="2">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:4">
       <c r="A76" s="2">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:4">
       <c r="A77" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B77" s="2">
         <v>4</v>
@@ -1042,9 +1095,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:4">
       <c r="A78" s="2">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B78" s="2">
         <v>4</v>
@@ -1053,41 +1106,41 @@
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:4">
       <c r="A79" s="2">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B79" s="2">
         <v>4</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="2">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B83" s="2">
         <v>5</v>
@@ -1098,14 +1151,14 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B85" s="2">
         <v>5</v>
@@ -1116,7 +1169,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B86" s="2">
         <v>5</v>
@@ -1130,49 +1183,52 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
+      <c r="D90" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B93" s="2">
         <v>6</v>
@@ -1181,14 +1237,14 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B95" s="2">
         <v>7</v>
@@ -1199,7 +1255,7 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -1209,7 +1265,7 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -1219,21 +1275,21 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B100" s="2">
         <v>7</v>
@@ -1242,7 +1298,7 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -1252,84 +1308,84 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -1339,28 +1395,28 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B117" s="2">
         <v>7</v>
@@ -1371,7 +1427,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B118" s="2">
         <v>7</v>
@@ -1382,7 +1438,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B119" s="2">
         <v>8</v>
@@ -1393,21 +1449,21 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="2">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="2">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B122" s="2">
         <v>8</v>
@@ -1416,7 +1472,7 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B123" s="2">
         <v>8</v>
@@ -1425,28 +1481,28 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="2">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="2">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -1456,7 +1512,7 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="2">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B128" s="2">
         <v>8</v>
@@ -1465,255 +1521,278 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="2">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="2">
-        <v>187</v>
-      </c>
-      <c r="B130" s="2"/>
+        <v>185</v>
+      </c>
+      <c r="B130" s="2">
+        <v>8</v>
+      </c>
       <c r="C130" s="2"/>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" ht="11.5" customHeight="1">
       <c r="A131" s="2">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="2">
-        <v>189</v>
-      </c>
-      <c r="B132" s="2">
-        <v>8</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="B132" s="2"/>
       <c r="C132" s="2"/>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="2">
-        <v>190</v>
-      </c>
-      <c r="B133" s="2"/>
+        <v>188</v>
+      </c>
+      <c r="B133" s="2">
+        <v>8</v>
+      </c>
       <c r="C133" s="2"/>
-      <c r="D133" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="2">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
+      <c r="D134" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="2">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="2">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
-      <c r="D136" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="2">
-        <v>201</v>
-      </c>
-      <c r="B137" s="2">
-        <v>9</v>
-      </c>
-      <c r="C137" s="2">
-        <v>1</v>
+        <v>192</v>
+      </c>
+      <c r="B137" s="2"/>
+      <c r="C137" s="2"/>
+      <c r="D137" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="2">
-        <v>202</v>
-      </c>
-      <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
+        <v>193</v>
+      </c>
+      <c r="B138" s="2">
+        <v>9</v>
+      </c>
+      <c r="C138" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="2">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="2">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="2">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="2">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="2">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="2">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="2">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="2">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="2">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
-      <c r="D147" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="2">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
+      <c r="D148" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="2">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
-      <c r="D149" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="2">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
+      <c r="D150" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="2">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="2">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="2">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="2">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="2">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="2">
-        <v>221</v>
-      </c>
-      <c r="B156" s="2">
-        <v>9</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="B156" s="2"/>
       <c r="C156" s="2"/>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="2">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B157" s="2">
         <v>9</v>
       </c>
       <c r="C157" s="2"/>
-      <c r="D157" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="2">
-        <v>223</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="B158" s="2">
+        <v>9</v>
+      </c>
+      <c r="C158" s="2"/>
       <c r="D158" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="2">
-        <v>249</v>
+        <v>222</v>
+      </c>
+      <c r="D159" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="2">
-        <v>250</v>
+        <v>223</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="2">
+        <v>249</v>
+      </c>
+      <c r="B161">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="2">
+        <v>250</v>
+      </c>
+      <c r="B162">
+        <v>11</v>
+      </c>
+      <c r="D162" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="2">
         <v>251</v>
       </c>
-      <c r="D161" t="s">
+      <c r="B163">
         <v>11</v>
       </c>
     </row>

</xml_diff>